<commit_message>
added more element types
</commit_message>
<xml_diff>
--- a/assets/design/WRLDC Tables.xlsx
+++ b/assets/design/WRLDC Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7965" firstSheet="18" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7965" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Generating Station" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="248">
   <si>
     <t>Generating Station</t>
   </si>
@@ -790,6 +790,12 @@
   </si>
   <si>
     <t>FK(ElementType)</t>
+  </si>
+  <si>
+    <t>FilterBankNumber</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -2162,12 +2168,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" ht="12.75">
       <c r="B2" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" ht="12.75">
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
@@ -2680,6 +2686,7 @@
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FF00B050"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:C4"/>
@@ -2778,23 +2785,23 @@
   </sheetPr>
   <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" ht="12.75">
       <c r="B2" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" ht="12.75">
       <c r="B3" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" ht="12.75">
       <c r="B4" s="2" t="s">
         <v>216</v>
       </c>
@@ -2913,13 +2920,19 @@
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FF00B050"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B3:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
@@ -2928,10 +2941,10 @@
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -2974,6 +2987,7 @@
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FF00B050"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:C4"/>
@@ -3771,7 +3785,9 @@
   </sheetPr>
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>